<commit_message>
Function Generator With Voltage Converter
added images and edited description
</commit_message>
<xml_diff>
--- a/Function Generator With Voltage Converter/04-CALCULATIONS.xlsx
+++ b/Function Generator With Voltage Converter/04-CALCULATIONS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\Projekty, Schematy, Przepisy\026.MP.JW. - Generator Funkcji\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacek\Documents\GitHub\projects_uC_repo\Function Generator With Voltage Converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86E5EFA-373E-40C8-8206-B0A98405345A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6235014C-7021-4B50-A444-448FADDC08B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Offset" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>V2 [V]</t>
   </si>
@@ -168,6 +168,9 @@
   <si>
     <t>SQUARE</t>
   </si>
+  <si>
+    <t>OLD OFFSET MEASURE WAY</t>
+  </si>
 </sst>
 </file>
 
@@ -264,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -296,6 +299,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -305,9 +311,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -4196,19 +4200,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -5283,19 +5287,19 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -6564,8 +6568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379293A-06FC-47F6-B029-F22B9121D69C}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6617,7 +6621,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="8"/>
       <c r="D4" s="7" t="s">
         <v>8</v>
@@ -6627,7 +6631,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="8"/>
       <c r="D5" s="7" t="s">
         <v>10</v>
@@ -6637,67 +6641,76 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="8"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="8"/>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+    </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="8"/>
     </row>
   </sheetData>
@@ -6709,10 +6722,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138EF8CC-60FC-49C5-9F2E-B3CAE7D67094}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6932,6 +6945,11 @@
       <c r="C18" s="11">
         <f t="shared" si="0"/>
         <v>1.005586592178771</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -6955,7 +6973,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -6973,15 +6991,15 @@
       <c r="F1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
@@ -6997,8 +7015,8 @@
       <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
@@ -7410,13 +7428,13 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="7" t="s">
         <v>26</v>
       </c>
@@ -7842,13 +7860,13 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="7" t="s">
         <v>27</v>
       </c>

</xml_diff>